<commit_message>
FILE NAMES and a lot of tweeks
FILE NAMES and a lot of tweeks
</commit_message>
<xml_diff>
--- a/upgrade_tasks/latestProactiveCheck_TestCases.xlsx
+++ b/upgrade_tasks/latestProactiveCheck_TestCases.xlsx
@@ -413,7 +413,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,9 +537,13 @@
         <v>4</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="H4" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="J4" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
@@ -561,9 +565,13 @@
         <v>5</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="H5" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="J5" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -715,9 +723,13 @@
         <v>17</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="H11" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="J11" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">

</xml_diff>